<commit_message>
director schedule handler function added admin file handler bug fix (when not log user write text, not /start) schedule_template.xlsx first version
</commit_message>
<xml_diff>
--- a/auxiliary/schedule_template.xlsx
+++ b/auxiliary/schedule_template.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26219"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9DFD31AE-A49C-44DA-983C-3D2A25DDB5D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4D4806B-6282-417E-A5BA-80E44A701D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,6 +27,44 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>Дата</t>
+  </si>
+  <si>
+    <t>День недели</t>
+  </si>
+  <si>
+    <t>Понедельник</t>
+  </si>
+  <si>
+    <t>Цвет</t>
+  </si>
+  <si>
+    <t>Время начала</t>
+  </si>
+  <si>
+    <t>Кабинет</t>
+  </si>
+  <si>
+    <t>Сод-ние</t>
+  </si>
+  <si>
+    <t>!</t>
+  </si>
+  <si>
+    <t>Карта</t>
+  </si>
+  <si>
+    <t>Врач</t>
+  </si>
+  <si>
+    <t>Пациент</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1">
@@ -46,10 +84,88 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -58,8 +174,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -374,12 +517,192 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" style="2"/>
+    <col min="2" max="2" width="13.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="2" customWidth="1"/>
+    <col min="7" max="8" width="30.7109375" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="10.7109375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="9">
+        <v>44984</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
admin file handler bug fix v2.0 (when not log user write text, not /start) schedule handler function in beta(print) version
</commit_message>
<xml_diff>
--- a/auxiliary/schedule_template.xlsx
+++ b/auxiliary/schedule_template.xlsx
@@ -3,12 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26219"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4D4806B-6282-417E-A5BA-80E44A701D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F2B3774-2134-4D68-9545-4862691D92E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Инструкция по пользованию" sheetId="3" r:id="rId1"/>
+    <sheet name="Газимов Игорь Грегорьевич" sheetId="1" r:id="rId2"/>
+    <sheet name="Шешенин Владимир Киприянович" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -28,7 +30,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="29">
+  <si>
+    <t>Дату нужно проставлять только в первый день недели, дальше оно проставится автоматически</t>
+  </si>
+  <si>
+    <t>Менять расположение ячеек в таблице СТРОГО ЗАПРЕЩЕНО, то есть редактировать ячейки можно начиная с 4 строки</t>
+  </si>
+  <si>
+    <t>Если необходимо записать пациента на следующую неделю или через несколько недель, то необходимо попросить у бота еще один шаблон рсписания и записывать пациента в нем, а когда наступит та неделя на которую вы записывали пациента, то просто отправить этот файл обратно боту</t>
+  </si>
   <si>
     <t>Дата</t>
   </si>
@@ -39,7 +50,25 @@
     <t>Понедельник</t>
   </si>
   <si>
-    <t>Цвет</t>
+    <t>Вторник</t>
+  </si>
+  <si>
+    <t>Среда</t>
+  </si>
+  <si>
+    <t>Четверг</t>
+  </si>
+  <si>
+    <t>Пятница</t>
+  </si>
+  <si>
+    <t>Суббота</t>
+  </si>
+  <si>
+    <t>Воскресенье</t>
+  </si>
+  <si>
+    <t>Категория</t>
   </si>
   <si>
     <t>Время начала</t>
@@ -51,16 +80,43 @@
     <t>Сод-ние</t>
   </si>
   <si>
-    <t>!</t>
+    <t>Комментарий</t>
   </si>
   <si>
     <t>Карта</t>
   </si>
   <si>
-    <t>Врач</t>
-  </si>
-  <si>
     <t>Пациент</t>
+  </si>
+  <si>
+    <t>QWE</t>
+  </si>
+  <si>
+    <t>Буба</t>
+  </si>
+  <si>
+    <t>Sheesh</t>
+  </si>
+  <si>
+    <t>ASD</t>
+  </si>
+  <si>
+    <t>Биба</t>
+  </si>
+  <si>
+    <t>Боба</t>
+  </si>
+  <si>
+    <t>BOOBA</t>
+  </si>
+  <si>
+    <t>)))</t>
+  </si>
+  <si>
+    <t>MLG</t>
+  </si>
+  <si>
+    <t>Boba2</t>
   </si>
 </sst>
 </file>
@@ -84,7 +140,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -170,19 +226,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -202,6 +268,15 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -516,191 +591,796 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2802D45F-D7A6-4D1A-9860-8B8228E7BD37}">
+  <dimension ref="A2:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:BC20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="2" customWidth="1"/>
+    <col min="3" max="4" width="8.7109375" style="2" customWidth="1"/>
+    <col min="5" max="6" width="13.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="2" customWidth="1"/>
+    <col min="11" max="12" width="8.7109375" style="2" customWidth="1"/>
+    <col min="13" max="14" width="13.7109375" style="2" customWidth="1"/>
+    <col min="15" max="15" width="30.7109375" style="2" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" style="2"/>
+    <col min="17" max="17" width="10.7109375" style="2" customWidth="1"/>
+    <col min="18" max="18" width="13.7109375" style="2" customWidth="1"/>
+    <col min="19" max="20" width="8.7109375" style="2" customWidth="1"/>
+    <col min="21" max="22" width="13.7109375" style="2" customWidth="1"/>
+    <col min="23" max="23" width="30.7109375" style="2" customWidth="1"/>
+    <col min="24" max="24" width="10.7109375" style="2"/>
+    <col min="25" max="25" width="10.7109375" style="2" customWidth="1"/>
+    <col min="26" max="26" width="13.7109375" style="2" customWidth="1"/>
+    <col min="27" max="28" width="8.7109375" style="2" customWidth="1"/>
+    <col min="29" max="30" width="13.7109375" style="2" customWidth="1"/>
+    <col min="31" max="31" width="30.7109375" style="2" customWidth="1"/>
+    <col min="32" max="32" width="10.7109375" style="2"/>
+    <col min="33" max="33" width="10.7109375" style="2" customWidth="1"/>
+    <col min="34" max="34" width="13.7109375" style="2" customWidth="1"/>
+    <col min="35" max="36" width="8.7109375" style="2" customWidth="1"/>
+    <col min="37" max="38" width="13.7109375" style="2" customWidth="1"/>
+    <col min="39" max="39" width="30.7109375" style="2" customWidth="1"/>
+    <col min="40" max="40" width="10.7109375" style="2"/>
+    <col min="41" max="41" width="10.7109375" style="2" customWidth="1"/>
+    <col min="42" max="42" width="13.7109375" style="2" customWidth="1"/>
+    <col min="43" max="44" width="8.7109375" style="2" customWidth="1"/>
+    <col min="45" max="46" width="13.7109375" style="2" customWidth="1"/>
+    <col min="47" max="47" width="30.7109375" style="2" customWidth="1"/>
+    <col min="48" max="48" width="10.7109375" style="2"/>
+    <col min="49" max="49" width="10.7109375" style="2" customWidth="1"/>
+    <col min="50" max="50" width="13.7109375" style="2" customWidth="1"/>
+    <col min="51" max="52" width="8.7109375" style="2" customWidth="1"/>
+    <col min="53" max="54" width="13.7109375" style="2" customWidth="1"/>
+    <col min="55" max="55" width="30.7109375" style="2" customWidth="1"/>
+    <col min="56" max="16384" width="10.7109375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:55">
+      <c r="A1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="I1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="Y1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AG1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI1" s="1"/>
+      <c r="AJ1" s="1"/>
+      <c r="AK1" s="1"/>
+      <c r="AL1" s="1"/>
+      <c r="AM1" s="1"/>
+      <c r="AO1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AP1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AQ1" s="1"/>
+      <c r="AR1" s="1"/>
+      <c r="AS1" s="1"/>
+      <c r="AT1" s="1"/>
+      <c r="AU1" s="1"/>
+      <c r="AW1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AX1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AY1" s="1"/>
+      <c r="AZ1" s="1"/>
+      <c r="BA1" s="1"/>
+      <c r="BB1" s="1"/>
+      <c r="BC1" s="1"/>
+    </row>
+    <row r="2" spans="1:55">
+      <c r="A2" s="8">
+        <v>44982</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="8">
+        <v>44985</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q2" s="8">
+        <v>44986</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y2" s="8">
+        <v>44987</v>
+      </c>
+      <c r="Z2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG2" s="8">
+        <v>44988</v>
+      </c>
+      <c r="AH2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AO2" s="8">
+        <v>44989</v>
+      </c>
+      <c r="AP2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AW2" s="8">
+        <v>44990</v>
+      </c>
+      <c r="AX2" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:55">
+      <c r="A3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="V3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="AG3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AI3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AK3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="AM3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="AO3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AQ3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AR3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AS3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AT3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="AU3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="AW3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AX3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AY3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AZ3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="BA3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="BB3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="BC3" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:55">
+      <c r="B4" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="2">
+        <v>123123</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AH4" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="AI4" s="2">
+        <v>2</v>
+      </c>
+      <c r="AJ4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AL4" s="2">
+        <v>123100</v>
+      </c>
+      <c r="AM4" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:55">
+      <c r="B5" s="11">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="2">
+        <v>123456</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:55">
+      <c r="B6" s="11">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="2">
+        <v>123789</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AX6" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="AY6" s="2">
+        <v>1337</v>
+      </c>
+      <c r="AZ6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="BA6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="BB6" s="2">
+        <v>13371337</v>
+      </c>
+      <c r="BC6" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20" s="11">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C20" s="2">
+        <v>2</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="2">
+        <v>678678</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC17DE14-1C8B-4E6F-B36A-0458C238EC85}">
+  <dimension ref="A1:BC3"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="13.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8" style="2" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="2" customWidth="1"/>
-    <col min="7" max="8" width="30.7109375" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="10.7109375" style="2"/>
+    <col min="3" max="4" width="8.7109375" style="2" customWidth="1"/>
+    <col min="5" max="6" width="13.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="2" customWidth="1"/>
+    <col min="11" max="12" width="8.7109375" style="2" customWidth="1"/>
+    <col min="13" max="14" width="13.7109375" style="2" customWidth="1"/>
+    <col min="15" max="15" width="30.7109375" style="2" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" style="2"/>
+    <col min="17" max="17" width="10.7109375" style="2" customWidth="1"/>
+    <col min="18" max="18" width="13.7109375" style="2" customWidth="1"/>
+    <col min="19" max="20" width="8.7109375" style="2" customWidth="1"/>
+    <col min="21" max="22" width="13.7109375" style="2" customWidth="1"/>
+    <col min="23" max="23" width="30.7109375" style="2" customWidth="1"/>
+    <col min="24" max="24" width="9.140625" style="2"/>
+    <col min="25" max="25" width="10.7109375" style="2" customWidth="1"/>
+    <col min="26" max="26" width="13.7109375" style="2" customWidth="1"/>
+    <col min="27" max="28" width="8.7109375" style="2" customWidth="1"/>
+    <col min="29" max="30" width="13.7109375" style="2" customWidth="1"/>
+    <col min="31" max="31" width="30.7109375" style="2" customWidth="1"/>
+    <col min="32" max="32" width="9.140625" style="2"/>
+    <col min="33" max="33" width="10.7109375" style="2" customWidth="1"/>
+    <col min="34" max="34" width="13.7109375" style="2" customWidth="1"/>
+    <col min="35" max="36" width="8.7109375" style="2" customWidth="1"/>
+    <col min="37" max="38" width="13.7109375" style="2" customWidth="1"/>
+    <col min="39" max="39" width="30.7109375" style="2" customWidth="1"/>
+    <col min="40" max="40" width="9.140625" style="2"/>
+    <col min="41" max="41" width="10.7109375" style="2" customWidth="1"/>
+    <col min="42" max="42" width="13.7109375" style="2" customWidth="1"/>
+    <col min="43" max="44" width="8.7109375" style="2" customWidth="1"/>
+    <col min="45" max="46" width="13.7109375" style="2" customWidth="1"/>
+    <col min="47" max="47" width="30.7109375" style="2" customWidth="1"/>
+    <col min="48" max="48" width="9.140625" style="2"/>
+    <col min="49" max="49" width="10.7109375" style="2" customWidth="1"/>
+    <col min="50" max="50" width="13.7109375" style="2" customWidth="1"/>
+    <col min="51" max="52" width="8.7109375" style="2" customWidth="1"/>
+    <col min="53" max="54" width="13.7109375" style="2" customWidth="1"/>
+    <col min="55" max="55" width="30.7109375" style="2" customWidth="1"/>
+    <col min="56" max="16384" width="10.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
+    <row r="1" spans="1:55">
+      <c r="A1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
+      <c r="I1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="Y1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AG1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI1" s="1"/>
+      <c r="AJ1" s="1"/>
+      <c r="AK1" s="1"/>
+      <c r="AL1" s="1"/>
+      <c r="AM1" s="1"/>
+      <c r="AO1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AP1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AQ1" s="1"/>
+      <c r="AR1" s="1"/>
+      <c r="AS1" s="1"/>
+      <c r="AT1" s="1"/>
+      <c r="AU1" s="1"/>
+      <c r="AW1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AX1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AY1" s="1"/>
+      <c r="AZ1" s="1"/>
+      <c r="BA1" s="1"/>
+      <c r="BB1" s="1"/>
+      <c r="BC1" s="1"/>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="9">
+    <row r="2" spans="1:55">
+      <c r="A2" s="8">
         <v>44984</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>2</v>
+      <c r="B2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="8">
+        <v>44985</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q2" s="8">
+        <v>44986</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y2" s="8">
+        <v>44987</v>
+      </c>
+      <c r="Z2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG2" s="8">
+        <v>44988</v>
+      </c>
+      <c r="AH2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AO2" s="8">
+        <v>44989</v>
+      </c>
+      <c r="AP2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AW2" s="8">
+        <v>44990</v>
+      </c>
+      <c r="AX2" s="7" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+    <row r="3" spans="1:55">
+      <c r="A3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="V3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="AG3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AI3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AK3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="AM3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="AO3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AQ3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AR3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AS3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AT3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="AU3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="AW3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AX3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AY3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AZ3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="BA3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="BB3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="BC3" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
schedule handler function without beauty output to message version 3.0 doctor schedule handler fully working
</commit_message>
<xml_diff>
--- a/auxiliary/schedule_template.xlsx
+++ b/auxiliary/schedule_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26219"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F2B3774-2134-4D68-9545-4862691D92E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FEA43588-5BFB-4336-8943-EF4F773C4621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -625,7 +625,7 @@
   <dimension ref="A1:BC20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
@@ -756,7 +756,7 @@
     </row>
     <row r="2" spans="1:55">
       <c r="A2" s="8">
-        <v>44982</v>
+        <v>44983</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>5</v>

</xml_diff>